<commit_message>
Rettet datofeil i test-kodebok
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/mrs5-kodebok/parse_kodebok_ok.xlsx
+++ b/tests/testthat/testdata/mrs5-kodebok/parse_kodebok_ok.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\endevj\OneDrive - Helse Vest\rapwhale\tests\testthat\testdata\mrs5-kodebok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA9E49E-2462-405C-BB11-02876D13E6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC40F5B4-0E2C-4BF5-BC96-AAC341A0D90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{532BB522-EB7E-4931-B041-1D7FE65AB65E}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="32">
   <si>
     <t>Skjematypenavn</t>
   </si>
@@ -134,7 +134,10 @@
     <t>Utskrevet</t>
   </si>
   <si>
-    <t>Versjon 3</t>
+    <t>01.03.2020 12:00</t>
+  </si>
+  <si>
+    <t>01.05.2021 12:00</t>
   </si>
 </sst>
 </file>
@@ -201,11 +204,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,7 +545,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C16" sqref="C16:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,8 +760,8 @@
       <c r="B17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="3">
-        <v>43831.5</v>
+      <c r="C17" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>10</v>
@@ -778,8 +780,8 @@
       <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="3">
-        <v>44197.5</v>
+      <c r="C18" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>12</v>
@@ -834,7 +836,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,8 +1050,8 @@
       <c r="B17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="3">
-        <v>43831.5</v>
+      <c r="C17" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>10</v>
@@ -1068,8 +1070,8 @@
       <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="3">
-        <v>44197.5</v>
+      <c r="C18" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>10</v>
@@ -1082,24 +1084,12 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>3</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="3">
-        <v>44562.5</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Oppdatert regler i test-kodebok
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/mrs5-kodebok/parse_kodebok_ok.xlsx
+++ b/tests/testthat/testdata/mrs5-kodebok/parse_kodebok_ok.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\endevj\OneDrive - Helse Vest\rapwhale\tests\testthat\testdata\mrs5-kodebok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5B0E75-A5EC-4112-94B4-50F87F578DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3407F2A-F6DB-49F8-A6E3-1B2EE5920419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{532BB522-EB7E-4931-B041-1D7FE65AB65E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{532BB522-EB7E-4931-B041-1D7FE65AB65E}"/>
   </bookViews>
   <sheets>
     <sheet name="Generelt" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="115">
   <si>
     <t>Skjematypenavn</t>
   </si>
@@ -368,9 +368,6 @@
     <t>Registerspesifikk validering</t>
   </si>
   <si>
-    <t>Innleggelsesdato kan ikke være senere enn utskrivningsdato som mangler på utskrivingsskjema.</t>
-  </si>
-  <si>
     <t>Skjul hvis</t>
   </si>
   <si>
@@ -378,6 +375,18 @@
   </si>
   <si>
     <t>Feltet (HoydeUkjent) er skjult hvis: Feltet (Hoyde) må besvares.</t>
+  </si>
+  <si>
+    <t>Feltet (Innlagt) må besvares.</t>
+  </si>
+  <si>
+    <t>Feltet (Innlagt) må være større enn eller lik 01.01.2020 00:00:00.</t>
+  </si>
+  <si>
+    <t>Feltet (Innlagt) må være mindre enn eller lik 16.04.2024 10:59:26.</t>
+  </si>
+  <si>
+    <t>Innleggelsesdato kan ikke være senere enn CreationDate.</t>
   </si>
 </sst>
 </file>
@@ -1045,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA42ACE6-2FE8-4E7C-A1D8-88580F11CF75}">
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,8 +1616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B76005-9B00-4617-936F-8E4E11920E3E}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1673,7 +1682,7 @@
         <v>97</v>
       </c>
       <c r="G2" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1708,7 +1717,7 @@
         <v>101</v>
       </c>
       <c r="G3" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1743,7 +1752,7 @@
         <v>105</v>
       </c>
       <c r="G4" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1772,13 +1781,13 @@
         <v>42</v>
       </c>
       <c r="E5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" t="s">
         <v>109</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>110</v>
-      </c>
-      <c r="G5" t="s">
-        <v>111</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1810,10 +1819,10 @@
         <v>107</v>
       </c>
       <c r="F6" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="G6" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="H6">
         <v>0</v>

</xml_diff>

<commit_message>
Rettet en feil i test-kodebok
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/mrs5-kodebok/parse_kodebok_ok.xlsx
+++ b/tests/testthat/testdata/mrs5-kodebok/parse_kodebok_ok.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://helsevest-my.sharepoint.com/personal/endevj_ihelse_net/Documents/rapwhale/tests/testthat/testdata/mrs5-kodebok/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\endevj\git-depot\rapwhale\tests\testthat\testdata\mrs5-kodebok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{5381A9A5-63C1-4237-89B0-698114071D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58C8D755-B21C-4D65-B66E-4E55B8278EE8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56AC1EF-1EEB-4AA8-A786-AAC76E03A2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="2" activeTab="6" xr2:uid="{532BB522-EB7E-4931-B041-1D7FE65AB65E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="2" activeTab="2" xr2:uid="{532BB522-EB7E-4931-B041-1D7FE65AB65E}"/>
   </bookViews>
   <sheets>
     <sheet name="Generelt" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="111">
   <si>
     <t>Skjematypenavn</t>
   </si>
@@ -463,9 +463,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -503,7 +503,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -609,7 +609,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -751,7 +751,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1040,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA42ACE6-2FE8-4E7C-A1D8-88580F11CF75}">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,28 +1295,28 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J6" t="s">
         <v>3</v>
@@ -1330,19 +1330,22 @@
       <c r="N6" t="s">
         <v>12</v>
       </c>
+      <c r="P6" t="s">
+        <v>73</v>
+      </c>
       <c r="U6" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
@@ -1372,27 +1375,27 @@
         <v>12</v>
       </c>
       <c r="P7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="U7" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G8" t="s">
         <v>12</v>
@@ -1416,24 +1419,24 @@
         <v>12</v>
       </c>
       <c r="P8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="U8" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E9" t="s">
         <v>54</v>
@@ -1460,7 +1463,7 @@
         <v>12</v>
       </c>
       <c r="P9" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="U9" t="s">
         <v>60</v>
@@ -1468,28 +1471,28 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J10" t="s">
         <v>3</v>
@@ -1503,28 +1506,25 @@
       <c r="N10" t="s">
         <v>12</v>
       </c>
-      <c r="P10" t="s">
-        <v>80</v>
-      </c>
       <c r="U10" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="D11" t="s">
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G11" t="s">
         <v>10</v>
@@ -1548,47 +1548,6 @@
         <v>12</v>
       </c>
       <c r="U11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I12">
-        <v>10</v>
-      </c>
-      <c r="J12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K12" t="s">
-        <v>3</v>
-      </c>
-      <c r="M12" t="s">
-        <v>12</v>
-      </c>
-      <c r="N12" t="s">
-        <v>12</v>
-      </c>
-      <c r="U12" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2669,7 +2628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0A829FA-5608-4069-A43E-FCC3E3B63B27}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>

</xml_diff>